<commit_message>
import employee no and leave type to excel file
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-leave-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-leave-template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="527"/>
+    <workbookView windowWidth="19890" windowHeight="8355" tabRatio="527"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="R E A D  M E  F I R S T" sheetId="5" r:id="rId2"/>
     <sheet name="E  X  A  M  P  L  E" sheetId="6" r:id="rId3"/>
+    <sheet name="Options" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
   <si>
     <t>Employee ID</t>
   </si>
@@ -27,6 +28,12 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Start Time (Optional)</t>
+  </si>
+  <si>
+    <t>End Time (Optional)</t>
+  </si>
+  <si>
     <t>Start Date</t>
   </si>
   <si>
@@ -60,15 +67,18 @@
     <t>detemines whether the user grants the leave or not</t>
   </si>
   <si>
-    <t>Start Time (Optional)</t>
-  </si>
-  <si>
-    <t>End Time (Optional)</t>
+    <t>the time when the filed leave begins. Leave it blank as long the user already provided the shift schedule in AccuPay</t>
+  </si>
+  <si>
+    <t>the time when the filed leave ends. Leave it blank as long the user already provided the shift schedule in AccuPay</t>
   </si>
   <si>
     <t>the date when the filed leave begins</t>
   </si>
   <si>
+    <t>the date when the filed leave ends. Leave it blank if value is the same as `Start Date`</t>
+  </si>
+  <si>
     <t>the explanation or notes why employee uses leave</t>
   </si>
   <si>
@@ -78,12 +88,12 @@
     <t>NOTE :</t>
   </si>
   <si>
+    <t>refer to the `E  X  A  M  P  L  E` worksheet</t>
+  </si>
+  <si>
     <t>worksheet name could be what ever the user desires</t>
   </si>
   <si>
-    <t>refer to the `E  X  A  M  P  L  E` worksheet</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -93,33 +103,31 @@
     <t>Approved</t>
   </si>
   <si>
+    <t>Family vacation</t>
+  </si>
+  <si>
     <t>Sick Leave</t>
   </si>
   <si>
-    <t>Family vacation</t>
-  </si>
-  <si>
     <t>not feeling well</t>
   </si>
   <si>
-    <t>the time when the filed leave begins. Leave it blank as long the user already provided the shift schedule in AccuPay</t>
-  </si>
-  <si>
-    <t>the time when the filed leave ends. Leave it blank as long the user already provided the shift schedule in AccuPay</t>
-  </si>
-  <si>
-    <t>the date when the filed leave ends. Leave it blank if value is the same as `Start Date`</t>
+    <t>EmployeeNo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,10 +136,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -139,33 +148,363 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -173,49 +512,341 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma 2" xfId="1"/>
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Comma 2" xfId="49"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <i val="0"/>
       </font>
       <fill>
@@ -527,198 +1158,204 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="41" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="12.8571428571429" style="13" customWidth="1"/>
+    <col min="2" max="2" width="22.8571428571429" style="13" customWidth="1"/>
+    <col min="3" max="3" width="12.8571428571429" style="13" customWidth="1"/>
+    <col min="4" max="4" width="19.8571428571429" style="14" customWidth="1"/>
+    <col min="5" max="5" width="19" style="14" customWidth="1"/>
+    <col min="6" max="7" width="21.4285714285714" style="15" customWidth="1"/>
+    <col min="8" max="8" width="32.5714285714286" style="13" customWidth="1"/>
+    <col min="9" max="9" width="41" style="13" customWidth="1"/>
+    <col min="10" max="10" width="25.5714285714286" style="16" customWidth="1"/>
+    <col min="11" max="11" width="22.4285714285714" style="16" customWidth="1"/>
+    <col min="12" max="12" width="6.57142857142857" style="16" customWidth="1"/>
+    <col min="13" max="16384" width="9.14285714285714" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection password="CD03" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
-      <formula1>"Leave w/o Pay,Maternity/paternity leave,Others,Sick leave,Vacation leave,Additional VL"</formula1>
+  <sheetProtection insertRows="0" deleteRows="0"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A$1:A$1048576">
+      <formula1>Options!$A$2:$A$1001</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576">
+      <formula1>Options!$B$2:$B$100</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C$1:C$1048576">
       <formula1>"Pending,Approved"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="23" style="10" customWidth="1"/>
-    <col min="2" max="2" width="105.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="23" style="8" customWidth="1"/>
+    <col min="2" max="2" width="105.857142857143" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9.14285714285714" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25">
+    <row r="1" ht="26.25" spans="1:2">
       <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="3" ht="32.25" customHeight="1" spans="1:2">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9"/>
-    </row>
-    <row r="3" spans="1:2" ht="32.25" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="B13" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="11"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>18</v>
+      <c r="B14" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>21</v>
+      <c r="A16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>20</v>
+      <c r="A17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -727,107 +1364,139 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="17.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="16.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="19.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="9.71428571428571" customWidth="1"/>
+    <col min="7" max="7" width="21.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="22.8571428571429" customWidth="1"/>
+    <col min="9" max="9" width="26.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="15">
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="7">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+1)</f>
-        <v>43563</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="8" t="s">
+        <v>43598</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="15">
+      <c r="B3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="7">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+2)</f>
-        <v>43564</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>27</v>
+        <v>43599</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection password="CD03" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"Leave w/o Pay,Maternity/paternity leave,Others,Sick leave,Vacation leave,Additional VL"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"Pending,Approved"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"Leave w/o Pay,Maternity/paternity leave,Others,Sick leave,Vacation leave,Additional VL"</formula1>
-    </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="14.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="18.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: leave import open to all
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-leave-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-leave-template.xlsx
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lambert\accupay\AccuPay\ImportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="VcWraKVfbOj4Z6kNTtAxr+P4OjNmepxK8LrNhbXppmuOZblu84XhCErCNsfnRAgpLATR2YIrucjhBDPhbwMifw==" workbookSaltValue="HhMOE8j7/JiukYhAd7nTHA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
@@ -15,7 +16,7 @@
     <sheet name="R E A D M E " sheetId="1" r:id="rId1"/>
     <sheet name="Employee Leave" sheetId="2" r:id="rId2"/>
     <sheet name="E  X  A  M  P  L  E" sheetId="3" r:id="rId3"/>
-    <sheet name="Options" sheetId="4" r:id="rId4"/>
+    <sheet name="Options" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>AccuPay Leave Import Template</t>
   </si>
@@ -164,6 +165,9 @@
   </si>
   <si>
     <t>EmployeeRowId</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -233,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
@@ -265,13 +269,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -567,16 +572,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="20"/>
     </row>
     <row r="3" spans="1:2" ht="32.25" customHeight="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="21"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
@@ -686,7 +691,8 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -732,7 +738,7 @@
       <c r="H1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -755,7 +761,7 @@
       <c r="F6" s="14"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tNCfMO1Hfr8vgv1pZiXaGBa5WoKFHLjU3TRN6mtOBbHJJZkf4VQRRwsyD1TA5svp2P9C1edCydly0UkluEpadw==" saltValue="VKqY6NXF7q4t6YKbWEbrgg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/lUaWjebebjMwD85WioKhoK95Su1+cDA8FiXd18gr87oRC3hbGk9kqa3lvrFc49LbJP/Kfubm9Q4siu+6pN6Ow==" saltValue="5WOoTVlXzg8KH1f8v68HAQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -765,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -821,7 +827,7 @@
       </c>
       <c r="D2" s="17">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+1)</f>
-        <v>45012</v>
+        <v>45019</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>28</v>
@@ -839,14 +845,14 @@
       </c>
       <c r="D3" s="17">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+2)</f>
-        <v>45013</v>
+        <v>45020</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="CD03" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="XurV3K1QuICvzB0UBaHLeKR/2QfZOZBK+B/DlLryQ9epkyvEPl0MrFpAjGPpDzg8zVAlGtiSjZ3J+U4uJo6oXQ==" saltValue="0L+yyIlEeLRT62wNpfHsHg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
       <formula1>"Leave w/o Pay,Maternity/paternity leave,Others,Sick leave,Vacation leave,Additional VL"</formula1>
@@ -858,15 +864,17 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
@@ -874,15 +882,29 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
+      <c r="D1" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="D2" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="D3" s="22" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="/5EUj4C4/cE84JhSwXD5nQEMxRL8Ba29JVnsMDtwqu3XsQBvO3g2vsSyecjicl7F/sqLljGIss56k4AAu9Ux4g==" saltValue="EhcOuDqeET1xvFJhrj1HiA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>